<commit_message>
mudanca nos nomes de entidades
</commit_message>
<xml_diff>
--- a/files/Banco de Dados/Dicionário de Dados.xlsx
+++ b/files/Banco de Dados/Dicionário de Dados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="113">
   <si>
     <t>Atributo</t>
   </si>
@@ -339,6 +339,30 @@
   </si>
   <si>
     <t>Identificador único do pedido</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>1~50</t>
+  </si>
+  <si>
+    <t>ingressante</t>
+  </si>
+  <si>
+    <t>Identificador único do ingresso no pedido</t>
+  </si>
+  <si>
+    <t>CPF do ingressante</t>
+  </si>
+  <si>
+    <t>E-mail do ingressante</t>
+  </si>
+  <si>
+    <t>Nome do ingressante</t>
+  </si>
+  <si>
+    <t>Entidade: ItemPedido</t>
   </si>
 </sst>
 </file>
@@ -381,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -651,11 +675,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,50 +786,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,30 +1172,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="46.42578125" style="6"/>
+    <col min="3" max="3" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="46.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1095,949 +1205,1107 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="29" t="s">
+      <c r="B9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="29"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="29"/>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="29"/>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="29"/>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="29"/>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="29"/>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="29"/>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="29"/>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="13"/>
+      <c r="E18" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="29"/>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="29"/>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="29"/>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="29"/>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="30"/>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="14"/>
+      <c r="E23" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="27"/>
+      <c r="D28" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="E28" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="25"/>
+      <c r="D32" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="25"/>
+      <c r="D35" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+    <row r="36" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="19"/>
-    </row>
-    <row r="39" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="20"/>
+      <c r="D40" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="E40" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="10" t="s">
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="11" t="s">
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="19"/>
-    </row>
-    <row r="46" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+    </row>
+    <row r="46" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="20"/>
+      <c r="D47" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="E47" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
+    <row r="48" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="26"/>
+      <c r="D48" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17" t="s">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="19"/>
-    </row>
-    <row r="51" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40"/>
+    </row>
+    <row r="51" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="20"/>
+      <c r="D52" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="21" t="s">
+      <c r="E52" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="27"/>
+      <c r="D53" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E53" s="18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="27"/>
+      <c r="D54" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="E54" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="25"/>
+      <c r="D55" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="E55" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="25"/>
+      <c r="D56" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="E56" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="25"/>
+      <c r="D57" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="25" t="s">
+    <row r="58" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="26"/>
+      <c r="D58" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="E58" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="19"/>
-    </row>
-    <row r="61" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="40"/>
+    </row>
+    <row r="61" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="27" t="s">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="20"/>
+      <c r="D62" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="21" t="s">
+      <c r="E62" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" s="27"/>
+      <c r="D63" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="E63" s="18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="27"/>
+      <c r="D64" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="E64" s="18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="25"/>
+      <c r="D65" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="E65" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
+    <row r="66" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B66" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="26"/>
+      <c r="D66" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="E66" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="17" t="s">
+    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="19"/>
-    </row>
-    <row r="69" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="38"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="40"/>
+    </row>
+    <row r="69" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="4"/>
+      <c r="D69" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="E69" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="27" t="s">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="20"/>
+      <c r="D70" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="21" t="s">
+      <c r="E70" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="25" t="s">
+    <row r="71" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="30" t="s">
+      <c r="C71" s="26"/>
+      <c r="D71" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="17" t="s">
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="19"/>
-    </row>
-    <row r="74" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="38"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="40"/>
+    </row>
+    <row r="74" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="4"/>
+      <c r="D74" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="27" t="s">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="20"/>
+      <c r="D75" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D75" s="21" t="s">
+      <c r="E75" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="23" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C76" s="31" t="s">
+      <c r="C76" s="27"/>
+      <c r="D76" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="22" t="s">
+      <c r="E76" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="28" t="s">
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
         <v>96</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="25"/>
+      <c r="D77" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="10" t="s">
+      <c r="E77" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="25" t="s">
+    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B78" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="30"/>
-      <c r="D78" s="11" t="s">
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="17" t="s">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="19"/>
-    </row>
-    <row r="81" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="38"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="40"/>
+    </row>
+    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="4"/>
+      <c r="D81" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="E81" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="27" t="s">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="24" t="s">
+      <c r="C82" s="20"/>
+      <c r="D82" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D82" s="21" t="s">
+      <c r="E82" s="17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="25" t="s">
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="30" t="s">
+      <c r="C83" s="26"/>
+      <c r="D83" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="E83" s="11" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B85" s="38"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="40"/>
+    </row>
+    <row r="86" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B89" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="11">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A68:E68"/>
   </mergeCells>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="1.1811023622047245" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removendo o tipo de ingresso
</commit_message>
<xml_diff>
--- a/files/Banco de Dados/Dicionário de Dados.xlsx
+++ b/files/Banco de Dados/Dicionário de Dados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
   <si>
     <t>Atributo</t>
   </si>
@@ -311,9 +311,6 @@
     <t>Data na qual o pedido foi realizado</t>
   </si>
   <si>
-    <t>Entidade: IngressoDisponivel</t>
-  </si>
-  <si>
     <t>quantidade</t>
   </si>
   <si>
@@ -329,15 +326,6 @@
     <t>Descrição do ingresso</t>
   </si>
   <si>
-    <t>Entidade: CategoriaIngresso</t>
-  </si>
-  <si>
-    <t>Nome da categoria do ingresso</t>
-  </si>
-  <si>
-    <t>Identificador único da categoria de ingresso</t>
-  </si>
-  <si>
     <t>Identificador único do pedido</t>
   </si>
   <si>
@@ -363,6 +351,9 @@
   </si>
   <si>
     <t>Entidade: ItemPedido</t>
+  </si>
+  <si>
+    <t>Entidade: TipoDeIngresso</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>71</v>
@@ -1237,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>73</v>
@@ -2057,7 +2048,7 @@
         <v>76</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2078,7 +2069,7 @@
     <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="37" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B73" s="38"/>
       <c r="C73" s="39"/>
@@ -2112,200 +2103,155 @@
         <v>76</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="18"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27" t="s">
+      <c r="B77" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E76" s="18" t="s">
+      <c r="E77" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25" t="s">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="38"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="40"/>
+    </row>
+    <row r="82" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E77" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B80" s="38"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="40"/>
-    </row>
-    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E82" s="17" t="s">
+      <c r="E84" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="21" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" s="26"/>
-      <c r="D83" s="26" t="s">
+      <c r="B86" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E83" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B85" s="38"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="40"/>
-    </row>
-    <row r="86" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B88" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E88" s="36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B89" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="21" t="s">
+      <c r="E86" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B90" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>111</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A68:E68"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A73:E73"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A68:E68"/>
   </mergeCells>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="1.1811023622047245" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
remocao de atributos bancarios do administrador e criacao da conta adm
</commit_message>
<xml_diff>
--- a/files/Banco de Dados/Dicionário de Dados.xlsx
+++ b/files/Banco de Dados/Dicionário de Dados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="112">
   <si>
     <t>Atributo</t>
   </si>
@@ -272,15 +272,6 @@
     <t>E-mail do administrador</t>
   </si>
   <si>
-    <t>Banco do administrador</t>
-  </si>
-  <si>
-    <t>Agencia bancária do administrador</t>
-  </si>
-  <si>
-    <t>Conta bancária do administrador</t>
-  </si>
-  <si>
     <t>Nome do administrador</t>
   </si>
   <si>
@@ -354,6 +345,21 @@
   </si>
   <si>
     <t>Entidade: TipoDeIngresso</t>
+  </si>
+  <si>
+    <t>Entidade: ContaCaixaAdm</t>
+  </si>
+  <si>
+    <t>Valor que a conta possui</t>
+  </si>
+  <si>
+    <t>Banco da administração</t>
+  </si>
+  <si>
+    <t>Agencia bancária da administração</t>
+  </si>
+  <si>
+    <t>Conta bancária da administração</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -723,11 +729,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -847,6 +884,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1163,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>71</v>
@@ -1228,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>73</v>
@@ -1833,7 +1879,7 @@
         <v>73</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1851,407 +1897,453 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+    <row r="55" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="41"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="43"/>
+    </row>
+    <row r="57" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="40"/>
+    </row>
+    <row r="58" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25" t="s">
+      <c r="B60" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E55" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
+      <c r="E60" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25" t="s">
+      <c r="B61" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E61" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25" t="s">
+      <c r="B64" s="38"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="40"/>
+    </row>
+    <row r="65" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E67" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21" t="s">
+      <c r="B69" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B70" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26" t="s">
+      <c r="C70" s="26"/>
+      <c r="D70" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="40"/>
-    </row>
-    <row r="61" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="40"/>
+    </row>
+    <row r="73" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4" t="s">
+      <c r="C73" s="4"/>
+      <c r="D73" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B74" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20" t="s">
+      <c r="C74" s="20"/>
+      <c r="D74" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+      <c r="E74" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" s="38"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="40"/>
+    </row>
+    <row r="78" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27" t="s">
+      <c r="B80" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="18"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="E81" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="38"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="40"/>
+    </row>
+    <row r="86" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26" t="s">
+      <c r="B89" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="40"/>
-    </row>
-    <row r="69" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B73" s="38"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="40"/>
-    </row>
-    <row r="74" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E75" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="18"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B81" s="38"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="40"/>
-    </row>
-    <row r="82" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E83" s="17" t="s">
+      <c r="E90" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E84" s="36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A68:E68"/>
+  <mergeCells count="11">
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A72:E72"/>
   </mergeCells>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="1.1811023622047245" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>